<commit_message>
updated labs, recordings txt file
</commit_message>
<xml_diff>
--- a/Student/Modules/09_Security/Demo/DynamicRLS.xlsx
+++ b/Student/Modules/09_Security/Demo/DynamicRLS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PBI365\Student\Modules\09_Security\Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua.Hernandez\OneDrive - COMPAREX AG\Training\PBI365\Student\Modules\09_Security\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_1BD953C3752ADB64571A8DF9B9835F6F9BA3D19F" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{2B3752FA-9B41-4FD5-8F55-B8862DDDC414}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users Table" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
   <si>
     <t>User</t>
   </si>
@@ -108,11 +109,23 @@
   <si>
     <t>ODYSSEUS\TedP</t>
   </si>
+  <si>
+    <t>joshua.hernandez@comparex.com</t>
+  </si>
+  <si>
+    <t>Joshua Hernandez</t>
+  </si>
+  <si>
+    <t>student@baconrox.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>Josh BaconRox</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -165,6 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -223,35 +237,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Users" displayName="Users" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Users" displayName="Users" ref="A1:B13" totalsRowShown="0">
+  <autoFilter ref="A1:B13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="User"/>
-    <tableColumn id="2" name="UserName" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="User"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="UserName" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Regions" displayName="Regions" ref="A1:A4" totalsRowShown="0">
-  <autoFilter ref="A1:A4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Regions" displayName="Regions" ref="A1:A4" totalsRowShown="0">
+  <autoFilter ref="A1:A4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Region"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Region"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="UserRegion" displayName="UserRegion" ref="A1:B16" totalsRowShown="0">
-  <autoFilter ref="A1:B16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="UserRegion" displayName="UserRegion" ref="A1:B18" totalsRowShown="0">
+  <autoFilter ref="A1:B18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState ref="A2:B16">
     <sortCondition ref="A1:A16"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="User" dataDxfId="0"/>
-    <tableColumn id="2" name="Region"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="User" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Region"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -553,20 +567,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -582,7 +596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -590,7 +604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -598,7 +612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -606,7 +620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -614,7 +628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -622,7 +636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -630,7 +644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -638,7 +652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -646,7 +660,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -654,46 +668,64 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="AustinP@cpt0926.onmicrosoft.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="AustinP@cpt0926.onmicrosoft.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A12" r:id="rId2" xr:uid="{FDF58DC5-7610-47BE-AE87-628575D3CBAD}"/>
+    <hyperlink ref="A13" r:id="rId3" xr:uid="{5BE9B30C-A4CF-428D-9544-585A291BCE95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -707,20 +739,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -736,7 +768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -744,15 +776,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -760,15 +792,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -776,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -784,7 +816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -792,15 +824,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -808,7 +840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -816,7 +848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -824,15 +856,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -840,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -848,18 +880,40 @@
         <v>3</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="AustinP@cpt0926.onmicrosoft.com"/>
-    <hyperlink ref="A2" r:id="rId2" display="AustinP@cpt0926.onmicrosoft.com"/>
-    <hyperlink ref="A15" r:id="rId3" display="Student@cpt0926.onmicrosoft.com"/>
-    <hyperlink ref="A16" r:id="rId4" display="Student@cpt0926.onmicrosoft.com"/>
-    <hyperlink ref="A12" r:id="rId5" display="MaxwellS@cpt0926.onmicrosoft.com"/>
-    <hyperlink ref="A13" r:id="rId6" display="MaxwellS@cpt0926.onmicrosoft.com"/>
+    <hyperlink ref="A3" r:id="rId1" display="AustinP@cpt0926.onmicrosoft.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" display="AustinP@cpt0926.onmicrosoft.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A15" r:id="rId3" display="Student@cpt0926.onmicrosoft.com" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="A16" r:id="rId4" display="Student@cpt0926.onmicrosoft.com" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="A12" r:id="rId5" display="MaxwellS@cpt0926.onmicrosoft.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="A13" r:id="rId6" display="MaxwellS@cpt0926.onmicrosoft.com" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="A4" r:id="rId7" xr:uid="{E0CA7812-DF8E-4FEB-BA7E-5768AA1E8433}"/>
+    <hyperlink ref="A6" r:id="rId8" xr:uid="{E9277D06-7FDC-40FF-9A73-F7C7C570EFBF}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{942D0E37-359E-4A0A-8F5A-A4518B817F79}"/>
+    <hyperlink ref="A14" r:id="rId10" xr:uid="{E9DA0C15-2545-43AA-8231-68F737255F22}"/>
+    <hyperlink ref="A17" r:id="rId11" xr:uid="{29AEC63D-9A07-48CE-B1C3-55E8405A37D8}"/>
+    <hyperlink ref="A18" r:id="rId12" xr:uid="{EEC5A288-B819-447D-92EA-024718A659E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>